<commit_message>
Add message template logic and refactoring the StepFunction.
</commit_message>
<xml_diff>
--- a/contract_flow/CalloutBot.xlsx
+++ b/contract_flow/CalloutBot.xlsx
@@ -8,15 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyrus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BBB584-F729-4A63-9F65-63DE372AC4D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E209811-A8C3-4FDE-857B-EE52CE8B0F09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="639" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="639" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelLexBot" sheetId="5" r:id="rId1"/>
-    <sheet name="RepeatIntent" sheetId="8" r:id="rId2"/>
-    <sheet name="OkIntent" sheetId="6" r:id="rId3"/>
-    <sheet name="Option" sheetId="3" r:id="rId4"/>
+    <sheet name="OkIntent" sheetId="6" r:id="rId2"/>
+    <sheet name="YesIntent" sheetId="10" r:id="rId3"/>
+    <sheet name="NoIntent" sheetId="9" r:id="rId4"/>
+    <sheet name="AIntent" sheetId="11" r:id="rId5"/>
+    <sheet name="BIntent" sheetId="14" r:id="rId6"/>
+    <sheet name="CIntent" sheetId="13" r:id="rId7"/>
+    <sheet name="DIntent" sheetId="12" r:id="rId8"/>
+    <sheet name="EIntent" sheetId="15" r:id="rId9"/>
+    <sheet name="RepeatIntent" sheetId="8" r:id="rId10"/>
+    <sheet name="Option" sheetId="3" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="slotType">Option!$B$2:$B$95</definedName>
@@ -31,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="135">
   <si>
     <t>valueSelectionStrategy</t>
   </si>
@@ -384,23 +391,62 @@
     <t>Bot for callout</t>
   </si>
   <si>
-    <t>OK
-Yes
-Thank you
-I got it.</t>
-  </si>
-  <si>
-    <t>Intent for get the message.</t>
-  </si>
-  <si>
     <t>Intent for repeacting the message.</t>
   </si>
   <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Intent for OK.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Intent for Yes.</t>
+  </si>
+  <si>
+    <t>Intent for No.</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Intent for A.</t>
+  </si>
+  <si>
+    <t>Intent for B.</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Intent for C.</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Intent for D.</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Intent for E.</t>
+  </si>
+  <si>
     <t>Sorry
-No
 I don't understand it.
 Again
-Repeat</t>
+Repeat
+One more time</t>
   </si>
 </sst>
 </file>
@@ -753,7 +799,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853EA2F8-9DC1-4997-B76A-F5525605B581}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -817,7 +863,7 @@
         <v>97</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -843,7 +889,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -905,7 +951,520 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C95"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -930,7 +1489,7 @@
         <v>97</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -951,12 +1510,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1018,515 +1577,793 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C95"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC23F24-0250-4E80-B6C1-2FD5ED48C988}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>92</v>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9" xr:uid="{C13ED72D-74C0-4557-97EB-0DE198352BF8}">
+      <formula1>slotType</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{6AD9BA91-C45A-4A52-B2C0-1797C96A69B0}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{D2488CEF-5DF8-4A24-ACA1-6FA3B31AA944}">
+          <x14:formula1>
+            <xm:f>Option!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8119A331-D6FD-43E9-BBD0-ECB97C873FE5}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9" xr:uid="{60F8E904-A435-4D0C-A412-83F927BC6687}">
+      <formula1>slotType</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{59E3223A-2486-4770-879A-2F0C26F544EE}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{2B19FE66-C915-4283-A178-2E1823240F52}">
+          <x14:formula1>
+            <xm:f>Option!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEEAF87F-A5B1-47BD-AF27-597C59549289}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{32505B04-D159-43C7-9F25-6274A1251277}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9" xr:uid="{4F9A3152-839A-4A9B-B929-0A44EE3C84EA}">
+      <formula1>slotType</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{3685F72C-E976-4119-8301-04D26103895F}">
+          <x14:formula1>
+            <xm:f>Option!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCBCD38-EAF7-4026-A593-6F491DD38EB2}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9" xr:uid="{B47B6A80-BAA3-46C1-B860-F685294CF8AE}">
+      <formula1>slotType</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{C8E65CCF-29F8-4837-97F5-2F6604EC9029}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{14D2E726-9F44-4980-966C-B95D4DDB8E35}">
+          <x14:formula1>
+            <xm:f>Option!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8019E9-738B-4E50-8C00-9762510255C3}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9" xr:uid="{A2047BA0-A245-4E17-8855-6EA3096FDA84}">
+      <formula1>slotType</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{AA2C82A8-3873-4293-A308-263809D090C6}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{6FCF6EED-BF84-4849-981D-B1A0D77E09D5}">
+          <x14:formula1>
+            <xm:f>Option!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F2CA93-E1B6-47B7-9F55-B428E6B51B9D}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9" xr:uid="{CF062784-1950-4565-A945-60E99DC92982}">
+      <formula1>slotType</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{7F5EC3EB-FACF-4656-8300-8947ABA19E1D}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{2EAE8433-ED42-4085-BCD0-C6A05A0B1DD6}">
+          <x14:formula1>
+            <xm:f>Option!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB24EB5E-90BF-486B-8B6D-C625F2C0B426}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{C272437A-3904-4878-93A4-9F2CB308C3C3}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9" xr:uid="{05D7EEB4-F712-4D66-B5A5-3B711363FF5A}">
+      <formula1>slotType</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{AA7EAFD0-EF82-4A1E-B6C3-F3D91B80F7B0}">
+          <x14:formula1>
+            <xm:f>Option!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change to use Failback Intent to capture error.
</commit_message>
<xml_diff>
--- a/contract_flow/CalloutBot.xlsx
+++ b/contract_flow/CalloutBot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyrus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E209811-A8C3-4FDE-857B-EE52CE8B0F09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583A6A24-7E65-4179-A061-D3717BB23EDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="639" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="639" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelLexBot" sheetId="5" r:id="rId1"/>
@@ -22,8 +22,9 @@
     <sheet name="CIntent" sheetId="13" r:id="rId7"/>
     <sheet name="DIntent" sheetId="12" r:id="rId8"/>
     <sheet name="EIntent" sheetId="15" r:id="rId9"/>
-    <sheet name="RepeatIntent" sheetId="8" r:id="rId10"/>
-    <sheet name="Option" sheetId="3" r:id="rId11"/>
+    <sheet name="AMAZONFallbackIntent" sheetId="16" r:id="rId10"/>
+    <sheet name="AMAZONRepeatIntent" sheetId="8" r:id="rId11"/>
+    <sheet name="Option" sheetId="3" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="slotType">Option!$B$2:$B$95</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="134">
   <si>
     <t>valueSelectionStrategy</t>
   </si>
@@ -328,9 +329,6 @@
     <t>Sorry, I'm not able to assist at this time</t>
   </si>
   <si>
-    <t>I didn't understand you, what would you like to do?</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -391,62 +389,72 @@
     <t>Bot for callout</t>
   </si>
   <si>
-    <t>Intent for repeacting the message.</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>Intent for OK.</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Intent for Yes.</t>
   </si>
   <si>
     <t>Intent for No.</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>Intent for A.</t>
   </si>
   <si>
     <t>Intent for B.</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>Intent for C.</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Intent for D.</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>Intent for E.</t>
   </si>
   <si>
-    <t>Sorry
-I don't understand it.
-Again
-Repeat
-One more time</t>
+    <t>No
+No No</t>
+  </si>
+  <si>
+    <t>A
+A A</t>
+  </si>
+  <si>
+    <t>B
+B B</t>
+  </si>
+  <si>
+    <t>C
+C C</t>
+  </si>
+  <si>
+    <t>D
+D D</t>
+  </si>
+  <si>
+    <t>E
+E E</t>
+  </si>
+  <si>
+    <t>Yes
+Yes I do
+Yes Yes
+oh yes
+yup</t>
+  </si>
+  <si>
+    <t>OK
+Ok OK
+okay
+okay okay
+Oh ok</t>
+  </si>
+  <si>
+    <t>Intent for repeating the message.</t>
+  </si>
+  <si>
+    <t>Intent for Fallback.</t>
   </si>
 </sst>
 </file>
@@ -798,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,15 +818,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>95</v>
@@ -826,10 +834,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -839,11 +844,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853EA2F8-9DC1-4997-B76A-F5525605B581}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A1AFF7-88CD-41FB-A2D0-6F8B9B7FBC58}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,15 +865,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -876,25 +881,23 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>134</v>
-      </c>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -903,25 +906,136 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{178B223D-06FA-4F5E-87BF-B03292C465A7}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9" xr:uid="{09B0217D-6838-40DA-8EA3-75A16B47FAD4}">
+      <formula1>slotType</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{05FB5E96-24A4-4CD9-A52D-44580B2862AF}">
+          <x14:formula1>
+            <xm:f>Option!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853EA2F8-9DC1-4997-B76A-F5525605B581}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -951,7 +1065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
@@ -1126,7 +1240,7 @@
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
@@ -1301,7 +1415,7 @@
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
@@ -1311,7 +1425,7 @@
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
@@ -1371,7 +1485,7 @@
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
@@ -1431,7 +1545,7 @@
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
@@ -1451,7 +1565,7 @@
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
@@ -1469,7 +1583,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,15 +1600,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -1502,25 +1616,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -1529,25 +1643,25 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1582,7 +1696,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,15 +1713,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -1615,25 +1729,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -1642,25 +1756,25 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1695,7 +1809,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,15 +1826,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -1728,25 +1842,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -1755,25 +1869,25 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1808,7 +1922,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,15 +1939,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -1841,25 +1955,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -1868,25 +1982,25 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1938,15 +2052,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -1954,25 +2068,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -1981,25 +2095,25 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2051,15 +2165,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -2067,25 +2181,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -2094,25 +2208,25 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2164,15 +2278,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -2180,25 +2294,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -2207,25 +2321,25 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2260,7 +2374,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,15 +2391,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -2293,25 +2407,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -2320,25 +2434,25 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for Number, Date and Time.
</commit_message>
<xml_diff>
--- a/contract_flow/CalloutBot.xlsx
+++ b/contract_flow/CalloutBot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyrus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrus/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583A6A24-7E65-4179-A061-D3717BB23EDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2452CC15-9DA4-0C4E-B641-6F18178900EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="639" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" tabRatio="639" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelLexBot" sheetId="5" r:id="rId1"/>
@@ -806,17 +806,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
@@ -824,7 +824,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
@@ -832,7 +832,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -851,19 +851,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -871,7 +871,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -879,32 +879,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -962,19 +962,19 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -982,7 +982,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -990,32 +990,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -1069,18 +1069,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1113,462 +1113,462 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>92</v>
       </c>
@@ -1586,19 +1586,19 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -1614,17 +1614,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -1632,16 +1632,16 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -1699,19 +1699,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -1727,17 +1727,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -1745,16 +1745,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -1812,19 +1812,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -1840,17 +1840,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -1858,16 +1858,16 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -1921,23 +1921,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEEAF87F-A5B1-47BD-AF27-597C59549289}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -1953,17 +1953,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -1971,16 +1971,16 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -2038,19 +2038,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -2066,17 +2066,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -2084,16 +2084,16 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -2151,19 +2151,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -2179,17 +2179,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -2197,16 +2197,16 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -2264,19 +2264,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -2292,17 +2292,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -2310,16 +2310,16 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -2377,19 +2377,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="55.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>96</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -2405,17 +2405,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -2423,16 +2423,16 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>

</xml_diff>